<commit_message>
Galette V7.8 plugin Subscription V1.4
correction du bug #59 et mise à jour de table.xlsx
</commit_message>
<xml_diff>
--- a/doc/tables.xlsx
+++ b/doc/tables.xlsx
@@ -16,17 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>date_demande</t>
   </si>
   <si>
-    <t>somme_due</t>
-  </si>
-  <si>
-    <t>somme_payee</t>
-  </si>
-  <si>
     <t>price1</t>
   </si>
   <si>
@@ -142,6 +136,18 @@
   </si>
   <si>
     <t>feedback_act_off</t>
+  </si>
+  <si>
+    <t>0=en cours</t>
+  </si>
+  <si>
+    <t>1=validé</t>
+  </si>
+  <si>
+    <t>2=payé</t>
+  </si>
+  <si>
+    <t>3=refusé</t>
   </si>
 </sst>
 </file>
@@ -748,7 +754,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A8" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A6" totalsRowShown="0" dataDxfId="1">
   <tableColumns count="1">
     <tableColumn id="1" name="subscriptions" dataDxfId="0"/>
   </tableColumns>
@@ -1041,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1057,35 +1063,35 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1093,156 +1099,167 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G7" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="G8" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="D9" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="D10" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="G11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="D14" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="G18" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>41</v>
+      <c r="I22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="I23" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>